<commit_message>
Combined the two datasets and operate spreading at the end
</commit_message>
<xml_diff>
--- a/waste_flow/extra_data_xls/treatment_to_full_name.xlsx
+++ b/waste_flow/extra_data_xls/treatment_to_full_name.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="27320" yWindow="2380" windowWidth="16540" windowHeight="10460" tabRatio="500"/>
+    <workbookView xWindow="480" yWindow="15740" windowWidth="22380" windowHeight="11320" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
   <si>
     <t>full_name</t>
   </si>
@@ -35,9 +35,6 @@
     <t>category</t>
   </si>
   <si>
-    <t>DSP_L_OTH</t>
-  </si>
-  <si>
     <t>DSP_L</t>
   </si>
   <si>
@@ -53,15 +50,6 @@
     <t>RCV_R_B</t>
   </si>
   <si>
-    <t>RCV_R</t>
-  </si>
-  <si>
-    <t>RCV_B</t>
-  </si>
-  <si>
-    <t>Disposal - landfill and other (D1-D7, D12)</t>
-  </si>
-  <si>
     <t>Disposal - landfill (D1, D5, D12)</t>
   </si>
   <si>
@@ -75,12 +63,6 @@
   </si>
   <si>
     <t>Recovery - recycling and backfilling (R2-R11)</t>
-  </si>
-  <si>
-    <t>Recovery - recycling</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Recovery - backfilling </t>
   </si>
   <si>
     <t>disposal</t>
@@ -453,10 +435,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D22"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="134" zoomScaleNormal="134" zoomScalePageLayoutView="134" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="A7" sqref="A7:XFD8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -469,7 +451,7 @@
   <sheetData>
     <row r="1" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>0</v>
@@ -484,10 +466,10 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -495,10 +477,10 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -506,10 +488,10 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" t="s">
         <v>12</v>
-      </c>
-      <c r="C4" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -517,10 +499,10 @@
         <v>5</v>
       </c>
       <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" t="s">
         <v>13</v>
-      </c>
-      <c r="C5" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -528,50 +510,17 @@
         <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C6" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" t="s">
-        <v>15</v>
-      </c>
-      <c r="C7" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" t="s">
-        <v>16</v>
-      </c>
-      <c r="C8" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9" t="s">
-        <v>17</v>
-      </c>
-      <c r="C9" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B21" s="1"/>
-    </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B22" s="2"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B18" s="1"/>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B19" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update coefficients with Carla
</commit_message>
<xml_diff>
--- a/waste_flow/extra_data_xls/treatment_to_full_name.xlsx
+++ b/waste_flow/extra_data_xls/treatment_to_full_name.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="15740" windowWidth="22380" windowHeight="11320" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="51120" windowHeight="17340" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -438,7 +438,7 @@
   <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="134" zoomScaleNormal="134" zoomScalePageLayoutView="134" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:XFD8"/>
+      <selection activeCell="N19" sqref="N19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Have all lines for each waste category in outputs
</commit_message>
<xml_diff>
--- a/waste_flow/extra_data_xls/treatment_to_full_name.xlsx
+++ b/waste_flow/extra_data_xls/treatment_to_full_name.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="51120" windowHeight="17340" tabRatio="500"/>
+    <workbookView xWindow="24920" yWindow="460" windowWidth="19220" windowHeight="9360" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -438,13 +438,13 @@
   <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="134" zoomScaleNormal="134" zoomScalePageLayoutView="134" workbookViewId="0">
-      <selection activeCell="N19" sqref="N19"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15.83203125" customWidth="1"/>
-    <col min="2" max="2" width="63.83203125" customWidth="1"/>
+    <col min="2" max="2" width="50.33203125" customWidth="1"/>
     <col min="3" max="3" width="14.5" customWidth="1"/>
     <col min="4" max="4" width="12" customWidth="1"/>
   </cols>

</xml_diff>